<commit_message>
test script retry upon exception implemented.
</commit_message>
<xml_diff>
--- a/test_scripts/chrome/QS003_testscript.xlsx
+++ b/test_scripts/chrome/QS003_testscript.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\edge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\chrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8EA871-D9E4-4C9D-B03C-93809218BECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE2776A-BB83-492F-A70F-687EDBD3CD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
+    <workbookView xWindow="3972" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>wait_for_seconds</t>
   </si>
   <si>
-    <t>ThemeRoller: jQuery UI's theme builder application</t>
-  </si>
-  <si>
     <t>QS003</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>tool tip</t>
+  </si>
+  <si>
+    <t>THAT'S WHAT THIS WIDGET IS</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -596,10 +596,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -607,10 +607,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -618,10 +618,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -632,7 +632,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -640,10 +640,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -659,13 +659,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -678,16 +678,16 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- Added a new function `check_page_accessibility` to validate web page accessibility using axe-core. - Updated the `execute_test_script` function to include the new accessibility check keyword.
</commit_message>
<xml_diff>
--- a/test_scripts/chrome/QS003_testscript.xlsx
+++ b/test_scripts/chrome/QS003_testscript.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\chrome\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\allprojects\web_automation_htmltopdf\test_scripts\edge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE2776A-BB83-492F-A70F-687EDBD3CD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEBDC95-B4C8-45F0-A490-EB3E0DB068ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3972" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4369D99C-3FCA-451D-9ADF-0150CDA12363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>open_browser</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>THAT'S WHAT THIS WIDGET IS</t>
+  </si>
+  <si>
+    <t>check_page_accessibility</t>
+  </si>
+  <si>
+    <t>Check page is accesibility compliant</t>
+  </si>
+  <si>
+    <t>The page should be accesibility compliant</t>
   </si>
 </sst>
 </file>
@@ -516,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3916CC0C-2E25-4DCF-A97F-45AF0FE46343}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,32 +605,28 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -629,10 +634,10 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -640,68 +645,84 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>30</v>
+      <c r="A13" t="s">
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>35</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-    </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
     </row>
@@ -722,17 +743,20 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
-      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D31" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D33" s="4"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="4"/>
@@ -741,25 +765,28 @@
       <c r="D37" s="4"/>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D40" s="5"/>
+      <c r="D39" s="4"/>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="5"/>
     </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D42" s="5"/>
+    </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D43" s="4"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D46" s="4"/>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D49" s="5"/>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="4"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>